<commit_message>
fixed error importing parties
</commit_message>
<xml_diff>
--- a/NewYearStickers/Extraction/NewYearMenu.xlsx
+++ b/NewYearStickers/Extraction/NewYearMenu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hotso\source\repos\NewYearStickers\NewYearStickers\Extraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31B2B402-6CF4-4C31-92DA-9727386D90E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B314C4F4-E72D-4221-9D5B-46544A30FA90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hold" sheetId="1" r:id="rId1"/>
@@ -118,9 +118,6 @@
     <t>Fisk I lag</t>
   </si>
   <si>
-    <t>fiskesause /m safran</t>
-  </si>
-  <si>
     <t>Fjerkræ ballotine</t>
   </si>
   <si>
@@ -146,6 +143,9 @@
   </si>
   <si>
     <t>Vanilje is</t>
+  </si>
+  <si>
+    <t>fiskesause m safran</t>
   </si>
 </sst>
 </file>
@@ -519,7 +519,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -1647,8 +1647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C56D55F4-0A50-47F2-AA4D-226D4D8DCF2E}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1705,13 +1705,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F2">
         <v>175</v>
@@ -1723,7 +1723,7 @@
         <v>60</v>
       </c>
       <c r="I2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -1731,13 +1731,13 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B3">
         <v>50</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F3">
         <v>60</v>
@@ -1749,7 +1749,7 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -1757,13 +1757,13 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F4">
         <v>70</v>
       </c>
       <c r="I4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J4">
         <v>30</v>
@@ -1771,7 +1771,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F5">
         <v>200</v>
@@ -1779,7 +1779,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F6">
         <v>100</v>

</xml_diff>